<commit_message>
modelo treinado, e inicio dos testes de precisão
</commit_message>
<xml_diff>
--- a/documents/classes.xlsx
+++ b/documents/classes.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Semeq\Desktop\chats\chatbot_hipotese\documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Semeq\Desktop\chatbot_hipotese\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A274A3C-E99F-4E12-8B24-582712604E2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACC7573B-07FC-4238-BE69-D9E3C7D19756}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{C1190393-C72C-499D-B5C0-42E370606FD0}"/>
   </bookViews>
@@ -521,8 +521,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CFBE2DD-D146-4E4B-B18A-FC4693C24B24}">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>